<commit_message>
chore: sample data 추가
</commit_message>
<xml_diff>
--- a/resources/sample.xlsx
+++ b/resources/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CTR\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pyeong.oh/Desktop/Practice/Selenium-Crawling/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6299B11-B0B4-4EC6-8100-0052D471F037}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6F8C45-9DAA-5842-9CFE-10C31645D234}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{A56D77BE-17AE-4AA6-8B08-934F11A62FEA}"/>
+    <workbookView xWindow="19880" yWindow="2800" windowWidth="26160" windowHeight="17560" xr2:uid="{A56D77BE-17AE-4AA6-8B08-934F11A62FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="인풋 인덱스" sheetId="1" r:id="rId1"/>
@@ -11726,7 +11726,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11848,6 +11848,14 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -12021,7 +12029,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -12125,6 +12133,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -12444,23 +12455,23 @@
   <dimension ref="B1:H421"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="0" style="9" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="9"/>
     <col min="3" max="3" width="9" style="11"/>
-    <col min="4" max="4" width="11.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="31.75" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="6" customFormat="1" ht="20.25" thickBot="1">
+    <row r="1" spans="2:8" s="6" customFormat="1" ht="20" thickBot="1">
       <c r="B1" s="27" t="s">
         <v>440</v>
       </c>
@@ -12483,7 +12494,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="17.25" thickTop="1">
+    <row r="2" spans="2:8" ht="19" thickTop="1">
       <c r="B2" s="7" t="s">
         <v>442</v>
       </c>
@@ -12506,7 +12517,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" ht="18">
       <c r="B3" s="7" t="s">
         <v>443</v>
       </c>
@@ -12529,7 +12540,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" ht="18">
       <c r="B4" s="7" t="s">
         <v>444</v>
       </c>
@@ -12552,7 +12563,7 @@
         <v>9621</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" ht="18">
       <c r="B5" s="7" t="s">
         <v>445</v>
       </c>
@@ -12575,7 +12586,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" ht="18">
       <c r="B6" s="7" t="s">
         <v>446</v>
       </c>
@@ -12598,7 +12609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" ht="18">
       <c r="B7" s="7" t="s">
         <v>447</v>
       </c>
@@ -12621,7 +12632,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" ht="18">
       <c r="B8" s="7" t="s">
         <v>448</v>
       </c>
@@ -12644,7 +12655,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" ht="18">
       <c r="B9" s="7" t="s">
         <v>449</v>
       </c>
@@ -12667,7 +12678,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="18">
       <c r="B10" s="7" t="s">
         <v>450</v>
       </c>
@@ -12690,7 +12701,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" ht="18">
       <c r="B11" s="7" t="s">
         <v>451</v>
       </c>
@@ -12713,7 +12724,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" ht="18">
       <c r="B12" s="7" t="s">
         <v>452</v>
       </c>
@@ -12736,7 +12747,7 @@
         <v>9624</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" ht="18">
       <c r="B13" s="7" t="s">
         <v>453</v>
       </c>
@@ -12759,7 +12770,7 @@
         <v>9625</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="18">
       <c r="B14" s="7" t="s">
         <v>454</v>
       </c>
@@ -12782,7 +12793,7 @@
         <v>9630</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" ht="18">
       <c r="B15" s="7" t="s">
         <v>455</v>
       </c>
@@ -12805,7 +12816,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" ht="18">
       <c r="B16" s="7" t="s">
         <v>456</v>
       </c>
@@ -12828,7 +12839,7 @@
         <v>9622</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" ht="18">
       <c r="B17" s="7" t="s">
         <v>457</v>
       </c>
@@ -12851,7 +12862,7 @@
         <v>9459</v>
       </c>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" ht="18">
       <c r="B18" s="7" t="s">
         <v>458</v>
       </c>
@@ -12874,7 +12885,7 @@
         <v>9635</v>
       </c>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" ht="18">
       <c r="B19" s="7" t="s">
         <v>459</v>
       </c>
@@ -12897,7 +12908,7 @@
         <v>9632</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" ht="18">
       <c r="B20" s="7" t="s">
         <v>460</v>
       </c>
@@ -12920,7 +12931,7 @@
         <v>9620</v>
       </c>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" ht="18">
       <c r="B21" s="7" t="s">
         <v>461</v>
       </c>
@@ -12943,7 +12954,7 @@
         <v>9640</v>
       </c>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" ht="18">
       <c r="B22" s="7" t="s">
         <v>462</v>
       </c>
@@ -12966,7 +12977,7 @@
         <v>9612</v>
       </c>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" ht="18">
       <c r="B23" s="7" t="s">
         <v>463</v>
       </c>
@@ -12989,7 +13000,7 @@
         <v>9616</v>
       </c>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" ht="18">
       <c r="B24" s="7" t="s">
         <v>464</v>
       </c>
@@ -13012,7 +13023,7 @@
         <v>9613</v>
       </c>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" ht="18">
       <c r="B25" s="7" t="s">
         <v>465</v>
       </c>
@@ -13035,7 +13046,7 @@
         <v>9642</v>
       </c>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" ht="18">
       <c r="B26" s="7" t="s">
         <v>466</v>
       </c>
@@ -13058,7 +13069,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" ht="18">
       <c r="B27" s="7" t="s">
         <v>467</v>
       </c>
@@ -13081,7 +13092,7 @@
         <v>9618</v>
       </c>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" ht="18">
       <c r="B28" s="7" t="s">
         <v>468</v>
       </c>
@@ -13104,7 +13115,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" ht="18">
       <c r="B29" s="7" t="s">
         <v>469</v>
       </c>
@@ -13127,7 +13138,7 @@
         <v>9615</v>
       </c>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" ht="18">
       <c r="B30" s="7" t="s">
         <v>470</v>
       </c>
@@ -13150,7 +13161,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" ht="18">
       <c r="B31" s="7" t="s">
         <v>471</v>
       </c>
@@ -13173,7 +13184,7 @@
         <v>9623</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" ht="18">
       <c r="B32" s="7" t="s">
         <v>472</v>
       </c>
@@ -13196,7 +13207,7 @@
         <v>9641</v>
       </c>
     </row>
-    <row r="33" spans="2:8">
+    <row r="33" spans="2:8" ht="18">
       <c r="B33" s="7" t="s">
         <v>473</v>
       </c>
@@ -13219,7 +13230,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="2:8">
+    <row r="34" spans="2:8" ht="18">
       <c r="B34" s="7" t="s">
         <v>474</v>
       </c>
@@ -13242,7 +13253,7 @@
         <v>9610</v>
       </c>
     </row>
-    <row r="35" spans="2:8">
+    <row r="35" spans="2:8" ht="18">
       <c r="B35" s="7" t="s">
         <v>475</v>
       </c>
@@ -13265,7 +13276,7 @@
         <v>9643</v>
       </c>
     </row>
-    <row r="36" spans="2:8">
+    <row r="36" spans="2:8" ht="18">
       <c r="B36" s="7" t="s">
         <v>476</v>
       </c>
@@ -13288,7 +13299,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="37" spans="2:8">
+    <row r="37" spans="2:8" ht="18">
       <c r="B37" s="7" t="s">
         <v>477</v>
       </c>
@@ -13311,7 +13322,7 @@
         <v>9614</v>
       </c>
     </row>
-    <row r="38" spans="2:8">
+    <row r="38" spans="2:8" ht="18">
       <c r="B38" s="7" t="s">
         <v>478</v>
       </c>
@@ -13334,7 +13345,7 @@
         <v>9450</v>
       </c>
     </row>
-    <row r="39" spans="2:8">
+    <row r="39" spans="2:8" ht="18">
       <c r="B39" s="7" t="s">
         <v>479</v>
       </c>
@@ -13357,7 +13368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="2:8">
+    <row r="40" spans="2:8" ht="18">
       <c r="B40" s="7" t="s">
         <v>480</v>
       </c>
@@ -13380,7 +13391,7 @@
         <v>9646</v>
       </c>
     </row>
-    <row r="41" spans="2:8">
+    <row r="41" spans="2:8" ht="18">
       <c r="B41" s="7" t="s">
         <v>481</v>
       </c>
@@ -13403,7 +13414,7 @@
         <v>9644</v>
       </c>
     </row>
-    <row r="42" spans="2:8">
+    <row r="42" spans="2:8" ht="18">
       <c r="B42" s="7" t="s">
         <v>482</v>
       </c>
@@ -13426,7 +13437,7 @@
         <v>9645</v>
       </c>
     </row>
-    <row r="43" spans="2:8">
+    <row r="43" spans="2:8" ht="18">
       <c r="B43" s="7" t="s">
         <v>483</v>
       </c>
@@ -13449,7 +13460,7 @@
         <v>9647</v>
       </c>
     </row>
-    <row r="44" spans="2:8">
+    <row r="44" spans="2:8" ht="18">
       <c r="B44" s="7" t="s">
         <v>484</v>
       </c>
@@ -13472,7 +13483,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="45" spans="2:8">
+    <row r="45" spans="2:8" ht="18">
       <c r="B45" s="7" t="s">
         <v>485</v>
       </c>
@@ -13495,7 +13506,7 @@
         <v>1900153</v>
       </c>
     </row>
-    <row r="46" spans="2:8">
+    <row r="46" spans="2:8" ht="18">
       <c r="B46" s="7" t="s">
         <v>486</v>
       </c>
@@ -13518,7 +13529,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
+    <row r="47" spans="2:8" ht="18">
       <c r="B47" s="7" t="s">
         <v>487</v>
       </c>
@@ -13541,7 +13552,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="17.25" thickBot="1">
+    <row r="48" spans="2:8" ht="19" thickBot="1">
       <c r="B48" s="28" t="s">
         <v>488</v>
       </c>
@@ -13564,7 +13575,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="49" spans="4:8">
+    <row r="49" spans="4:8" ht="18">
       <c r="D49" s="12">
         <v>48</v>
       </c>
@@ -13581,7 +13592,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="50" spans="4:8">
+    <row r="50" spans="4:8" ht="18">
       <c r="D50" s="12">
         <v>49</v>
       </c>
@@ -13598,7 +13609,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="4:8">
+    <row r="51" spans="4:8" ht="18">
       <c r="D51" s="12">
         <v>50</v>
       </c>
@@ -13615,7 +13626,7 @@
         <v>5244</v>
       </c>
     </row>
-    <row r="52" spans="4:8">
+    <row r="52" spans="4:8" ht="18">
       <c r="D52" s="12">
         <v>51</v>
       </c>
@@ -13632,7 +13643,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="4:8">
+    <row r="53" spans="4:8" ht="18">
       <c r="D53" s="12">
         <v>52</v>
       </c>
@@ -13649,7 +13660,7 @@
         <v>1900147</v>
       </c>
     </row>
-    <row r="54" spans="4:8">
+    <row r="54" spans="4:8" ht="18">
       <c r="D54" s="12">
         <v>53</v>
       </c>
@@ -13666,7 +13677,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="4:8">
+    <row r="55" spans="4:8" ht="18">
       <c r="D55" s="12">
         <v>54</v>
       </c>
@@ -13683,7 +13694,7 @@
         <v>5326</v>
       </c>
     </row>
-    <row r="56" spans="4:8">
+    <row r="56" spans="4:8" ht="18">
       <c r="D56" s="12">
         <v>55</v>
       </c>
@@ -13700,7 +13711,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="57" spans="4:8">
+    <row r="57" spans="4:8" ht="18">
       <c r="D57" s="12">
         <v>56</v>
       </c>
@@ -13717,7 +13728,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="58" spans="4:8">
+    <row r="58" spans="4:8" ht="18">
       <c r="D58" s="12">
         <v>57</v>
       </c>
@@ -13734,7 +13745,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="59" spans="4:8">
+    <row r="59" spans="4:8" ht="18">
       <c r="D59" s="12">
         <v>58</v>
       </c>
@@ -13751,7 +13762,7 @@
         <v>4350</v>
       </c>
     </row>
-    <row r="60" spans="4:8">
+    <row r="60" spans="4:8" ht="18">
       <c r="D60" s="12">
         <v>59</v>
       </c>
@@ -13768,7 +13779,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="4:8">
+    <row r="61" spans="4:8" ht="18">
       <c r="D61" s="12">
         <v>60</v>
       </c>
@@ -13785,7 +13796,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="62" spans="4:8">
+    <row r="62" spans="4:8" ht="18">
       <c r="D62" s="12">
         <v>61</v>
       </c>
@@ -13802,7 +13813,7 @@
         <v>5342</v>
       </c>
     </row>
-    <row r="63" spans="4:8">
+    <row r="63" spans="4:8" ht="18">
       <c r="D63" s="12">
         <v>62</v>
       </c>
@@ -13819,7 +13830,7 @@
         <v>1900161</v>
       </c>
     </row>
-    <row r="64" spans="4:8">
+    <row r="64" spans="4:8" ht="18">
       <c r="D64" s="12">
         <v>63</v>
       </c>
@@ -13836,7 +13847,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="65" spans="4:8">
+    <row r="65" spans="4:8" ht="18">
       <c r="D65" s="12">
         <v>64</v>
       </c>
@@ -13853,7 +13864,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="66" spans="4:8">
+    <row r="66" spans="4:8" ht="18">
       <c r="D66" s="12">
         <v>65</v>
       </c>
@@ -13870,7 +13881,7 @@
         <v>1900170</v>
       </c>
     </row>
-    <row r="67" spans="4:8">
+    <row r="67" spans="4:8" ht="18">
       <c r="D67" s="12">
         <v>66</v>
       </c>
@@ -13887,7 +13898,7 @@
         <v>5786</v>
       </c>
     </row>
-    <row r="68" spans="4:8">
+    <row r="68" spans="4:8" ht="18">
       <c r="D68" s="12">
         <v>67</v>
       </c>
@@ -13904,7 +13915,7 @@
         <v>3276</v>
       </c>
     </row>
-    <row r="69" spans="4:8">
+    <row r="69" spans="4:8" ht="18">
       <c r="D69" s="12">
         <v>68</v>
       </c>
@@ -13921,7 +13932,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="4:8">
+    <row r="70" spans="4:8" ht="18">
       <c r="D70" s="12">
         <v>69</v>
       </c>
@@ -13938,7 +13949,7 @@
         <v>5277</v>
       </c>
     </row>
-    <row r="71" spans="4:8">
+    <row r="71" spans="4:8" ht="18">
       <c r="D71" s="12">
         <v>70</v>
       </c>
@@ -13955,7 +13966,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="72" spans="4:8">
+    <row r="72" spans="4:8" ht="18">
       <c r="D72" s="12">
         <v>71</v>
       </c>
@@ -13972,7 +13983,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="73" spans="4:8">
+    <row r="73" spans="4:8" ht="18">
       <c r="D73" s="12">
         <v>72</v>
       </c>
@@ -13989,7 +14000,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="74" spans="4:8">
+    <row r="74" spans="4:8" ht="18">
       <c r="D74" s="12">
         <v>73</v>
       </c>
@@ -14006,7 +14017,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="75" spans="4:8">
+    <row r="75" spans="4:8" ht="18">
       <c r="D75" s="12">
         <v>74</v>
       </c>
@@ -14023,7 +14034,7 @@
         <v>4435</v>
       </c>
     </row>
-    <row r="76" spans="4:8">
+    <row r="76" spans="4:8" ht="18">
       <c r="D76" s="12">
         <v>75</v>
       </c>
@@ -14040,7 +14051,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="77" spans="4:8">
+    <row r="77" spans="4:8" ht="18">
       <c r="D77" s="12">
         <v>76</v>
       </c>
@@ -14057,7 +14068,7 @@
         <v>1900145</v>
       </c>
     </row>
-    <row r="78" spans="4:8">
+    <row r="78" spans="4:8" ht="18">
       <c r="D78" s="12">
         <v>77</v>
       </c>
@@ -14074,7 +14085,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="79" spans="4:8">
+    <row r="79" spans="4:8" ht="18">
       <c r="D79" s="12">
         <v>78</v>
       </c>
@@ -14091,7 +14102,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="80" spans="4:8">
+    <row r="80" spans="4:8" ht="18">
       <c r="D80" s="12">
         <v>79</v>
       </c>
@@ -14108,7 +14119,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="81" spans="4:8">
+    <row r="81" spans="4:8" ht="18">
       <c r="D81" s="12">
         <v>80</v>
       </c>
@@ -14125,7 +14136,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="82" spans="4:8">
+    <row r="82" spans="4:8" ht="18">
       <c r="D82" s="12">
         <v>81</v>
       </c>
@@ -14142,7 +14153,7 @@
         <v>1900148</v>
       </c>
     </row>
-    <row r="83" spans="4:8">
+    <row r="83" spans="4:8" ht="18">
       <c r="D83" s="12">
         <v>82</v>
       </c>
@@ -14159,7 +14170,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="84" spans="4:8">
+    <row r="84" spans="4:8" ht="18">
       <c r="D84" s="12">
         <v>83</v>
       </c>
@@ -14176,7 +14187,7 @@
         <v>9554</v>
       </c>
     </row>
-    <row r="85" spans="4:8">
+    <row r="85" spans="4:8" ht="18">
       <c r="D85" s="12">
         <v>84</v>
       </c>
@@ -14193,7 +14204,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="86" spans="4:8">
+    <row r="86" spans="4:8" ht="18">
       <c r="D86" s="12">
         <v>85</v>
       </c>
@@ -14210,7 +14221,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="87" spans="4:8">
+    <row r="87" spans="4:8" ht="18">
       <c r="D87" s="12">
         <v>86</v>
       </c>
@@ -14227,7 +14238,7 @@
         <v>4437</v>
       </c>
     </row>
-    <row r="88" spans="4:8">
+    <row r="88" spans="4:8" ht="18">
       <c r="D88" s="12">
         <v>87</v>
       </c>
@@ -14244,7 +14255,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="89" spans="4:8">
+    <row r="89" spans="4:8" ht="18">
       <c r="D89" s="12">
         <v>88</v>
       </c>
@@ -14261,7 +14272,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="90" spans="4:8">
+    <row r="90" spans="4:8" ht="18">
       <c r="D90" s="12">
         <v>89</v>
       </c>
@@ -14278,7 +14289,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="91" spans="4:8">
+    <row r="91" spans="4:8" ht="18">
       <c r="D91" s="12">
         <v>90</v>
       </c>
@@ -14295,7 +14306,7 @@
         <v>1900151</v>
       </c>
     </row>
-    <row r="92" spans="4:8">
+    <row r="92" spans="4:8" ht="18">
       <c r="D92" s="12">
         <v>91</v>
       </c>
@@ -14312,7 +14323,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="93" spans="4:8">
+    <row r="93" spans="4:8" ht="18">
       <c r="D93" s="21">
         <v>92</v>
       </c>
@@ -14329,7 +14340,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="94" spans="4:8">
+    <row r="94" spans="4:8" ht="18">
       <c r="D94" s="12">
         <v>93</v>
       </c>
@@ -14346,7 +14357,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="4:8">
+    <row r="95" spans="4:8" ht="18">
       <c r="D95" s="12">
         <v>94</v>
       </c>
@@ -14363,7 +14374,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="4:8">
+    <row r="96" spans="4:8" ht="18">
       <c r="D96" s="12">
         <v>95</v>
       </c>
@@ -14380,7 +14391,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="4:8">
+    <row r="97" spans="4:8" ht="18">
       <c r="D97" s="12">
         <v>96</v>
       </c>
@@ -14397,7 +14408,7 @@
         <v>9536</v>
       </c>
     </row>
-    <row r="98" spans="4:8">
+    <row r="98" spans="4:8" ht="18">
       <c r="D98" s="12">
         <v>97</v>
       </c>
@@ -14414,7 +14425,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="99" spans="4:8">
+    <row r="99" spans="4:8" ht="18">
       <c r="D99" s="12">
         <v>98</v>
       </c>
@@ -14431,7 +14442,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="4:8">
+    <row r="100" spans="4:8" ht="18">
       <c r="D100" s="12">
         <v>99</v>
       </c>
@@ -14448,7 +14459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="4:8">
+    <row r="101" spans="4:8" ht="18">
       <c r="D101" s="12">
         <v>100</v>
       </c>
@@ -14465,7 +14476,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="4:8">
+    <row r="102" spans="4:8" ht="18">
       <c r="D102" s="12">
         <v>101</v>
       </c>
@@ -14482,7 +14493,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="103" spans="4:8">
+    <row r="103" spans="4:8" ht="18">
       <c r="D103" s="12">
         <v>102</v>
       </c>
@@ -14499,7 +14510,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" spans="4:8">
+    <row r="104" spans="4:8" ht="18">
       <c r="D104" s="12">
         <v>103</v>
       </c>
@@ -14516,7 +14527,7 @@
         <v>4058</v>
       </c>
     </row>
-    <row r="105" spans="4:8">
+    <row r="105" spans="4:8" ht="18">
       <c r="D105" s="12">
         <v>104</v>
       </c>
@@ -14533,7 +14544,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="106" spans="4:8">
+    <row r="106" spans="4:8" ht="18">
       <c r="D106" s="12">
         <v>105</v>
       </c>
@@ -14550,7 +14561,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="107" spans="4:8">
+    <row r="107" spans="4:8" ht="18">
       <c r="D107" s="12">
         <v>106</v>
       </c>
@@ -14567,7 +14578,7 @@
         <v>4048</v>
       </c>
     </row>
-    <row r="108" spans="4:8">
+    <row r="108" spans="4:8" ht="18">
       <c r="D108" s="12">
         <v>107</v>
       </c>
@@ -14584,7 +14595,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="109" spans="4:8">
+    <row r="109" spans="4:8" ht="18">
       <c r="D109" s="12">
         <v>108</v>
       </c>
@@ -14601,7 +14612,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="4:8">
+    <row r="110" spans="4:8" ht="18">
       <c r="D110" s="12">
         <v>109</v>
       </c>
@@ -14618,7 +14629,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="4:8">
+    <row r="111" spans="4:8" ht="18">
       <c r="D111" s="12">
         <v>110</v>
       </c>
@@ -14635,7 +14646,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="4:8">
+    <row r="112" spans="4:8" ht="18">
       <c r="D112" s="12">
         <v>111</v>
       </c>
@@ -14652,7 +14663,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="4:8">
+    <row r="113" spans="4:8" ht="18">
       <c r="D113" s="12">
         <v>112</v>
       </c>
@@ -14669,7 +14680,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="114" spans="4:8">
+    <row r="114" spans="4:8" ht="18">
       <c r="D114" s="12">
         <v>113</v>
       </c>
@@ -14686,7 +14697,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="115" spans="4:8">
+    <row r="115" spans="4:8" ht="18">
       <c r="D115" s="12">
         <v>114</v>
       </c>
@@ -14703,7 +14714,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="116" spans="4:8">
+    <row r="116" spans="4:8" ht="18">
       <c r="D116" s="12">
         <v>115</v>
       </c>
@@ -14720,7 +14731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="4:8">
+    <row r="117" spans="4:8" ht="18">
       <c r="D117" s="12">
         <v>116</v>
       </c>
@@ -14737,7 +14748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="118" spans="4:8">
+    <row r="118" spans="4:8" ht="18">
       <c r="D118" s="21">
         <v>117</v>
       </c>
@@ -14754,7 +14765,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="119" spans="4:8">
+    <row r="119" spans="4:8" ht="18">
       <c r="D119" s="12">
         <v>118</v>
       </c>
@@ -14771,7 +14782,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="120" spans="4:8">
+    <row r="120" spans="4:8" ht="18">
       <c r="D120" s="12">
         <v>119</v>
       </c>
@@ -14788,7 +14799,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="121" spans="4:8">
+    <row r="121" spans="4:8" ht="18">
       <c r="D121" s="12">
         <v>120</v>
       </c>
@@ -14805,7 +14816,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="4:8">
+    <row r="122" spans="4:8" ht="18">
       <c r="D122" s="12">
         <v>121</v>
       </c>
@@ -14822,7 +14833,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="4:8">
+    <row r="123" spans="4:8" ht="18">
       <c r="D123" s="12">
         <v>122</v>
       </c>
@@ -14839,7 +14850,7 @@
         <v>1900048</v>
       </c>
     </row>
-    <row r="124" spans="4:8">
+    <row r="124" spans="4:8" ht="18">
       <c r="D124" s="12">
         <v>123</v>
       </c>
@@ -14856,7 +14867,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="125" spans="4:8">
+    <row r="125" spans="4:8" ht="18">
       <c r="D125" s="12">
         <v>124</v>
       </c>
@@ -14873,7 +14884,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="4:8">
+    <row r="126" spans="4:8" ht="18">
       <c r="D126" s="12">
         <v>125</v>
       </c>
@@ -14890,7 +14901,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="127" spans="4:8">
+    <row r="127" spans="4:8" ht="18">
       <c r="D127" s="12">
         <v>126</v>
       </c>
@@ -14907,7 +14918,7 @@
         <v>3789</v>
       </c>
     </row>
-    <row r="128" spans="4:8">
+    <row r="128" spans="4:8" ht="18">
       <c r="D128" s="12">
         <v>127</v>
       </c>
@@ -14924,7 +14935,7 @@
         <v>1900039</v>
       </c>
     </row>
-    <row r="129" spans="4:8">
+    <row r="129" spans="4:8" ht="18">
       <c r="D129" s="12">
         <v>128</v>
       </c>
@@ -14941,7 +14952,7 @@
         <v>1900044</v>
       </c>
     </row>
-    <row r="130" spans="4:8">
+    <row r="130" spans="4:8" ht="18">
       <c r="D130" s="12">
         <v>129</v>
       </c>
@@ -14958,7 +14969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="4:8">
+    <row r="131" spans="4:8" ht="18">
       <c r="D131" s="12">
         <v>130</v>
       </c>
@@ -14975,7 +14986,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="132" spans="4:8">
+    <row r="132" spans="4:8" ht="18">
       <c r="D132" s="12">
         <v>131</v>
       </c>
@@ -14992,7 +15003,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="133" spans="4:8">
+    <row r="133" spans="4:8" ht="18">
       <c r="D133" s="12">
         <v>132</v>
       </c>
@@ -15009,7 +15020,7 @@
         <v>1900047</v>
       </c>
     </row>
-    <row r="134" spans="4:8">
+    <row r="134" spans="4:8" ht="18">
       <c r="D134" s="12">
         <v>133</v>
       </c>
@@ -15026,7 +15037,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="135" spans="4:8">
+    <row r="135" spans="4:8" ht="18">
       <c r="D135" s="12">
         <v>134</v>
       </c>
@@ -15043,7 +15054,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="136" spans="4:8">
+    <row r="136" spans="4:8" ht="18">
       <c r="D136" s="12">
         <v>135</v>
       </c>
@@ -15060,7 +15071,7 @@
         <v>1900061</v>
       </c>
     </row>
-    <row r="137" spans="4:8">
+    <row r="137" spans="4:8" ht="18">
       <c r="D137" s="12">
         <v>136</v>
       </c>
@@ -15077,7 +15088,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="138" spans="4:8">
+    <row r="138" spans="4:8" ht="18">
       <c r="D138" s="12">
         <v>137</v>
       </c>
@@ -15094,7 +15105,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="139" spans="4:8">
+    <row r="139" spans="4:8" ht="18">
       <c r="D139" s="12">
         <v>138</v>
       </c>
@@ -15111,7 +15122,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="140" spans="4:8">
+    <row r="140" spans="4:8" ht="18">
       <c r="D140" s="12">
         <v>139</v>
       </c>
@@ -15128,7 +15139,7 @@
         <v>9569</v>
       </c>
     </row>
-    <row r="141" spans="4:8">
+    <row r="141" spans="4:8" ht="18">
       <c r="D141" s="12">
         <v>140</v>
       </c>
@@ -15145,7 +15156,7 @@
         <v>2161</v>
       </c>
     </row>
-    <row r="142" spans="4:8">
+    <row r="142" spans="4:8" ht="18">
       <c r="D142" s="12">
         <v>141</v>
       </c>
@@ -15162,7 +15173,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="143" spans="4:8">
+    <row r="143" spans="4:8" ht="18">
       <c r="D143" s="12">
         <v>142</v>
       </c>
@@ -15179,7 +15190,7 @@
         <v>1900031</v>
       </c>
     </row>
-    <row r="144" spans="4:8">
+    <row r="144" spans="4:8" ht="18">
       <c r="D144" s="12">
         <v>143</v>
       </c>
@@ -15196,7 +15207,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="145" spans="4:8">
+    <row r="145" spans="4:8" ht="18">
       <c r="D145" s="12">
         <v>144</v>
       </c>
@@ -15213,7 +15224,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="146" spans="4:8">
+    <row r="146" spans="4:8" ht="18">
       <c r="D146" s="12">
         <v>145</v>
       </c>
@@ -15230,7 +15241,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="147" spans="4:8">
+    <row r="147" spans="4:8" ht="18">
       <c r="D147" s="12">
         <v>146</v>
       </c>
@@ -15247,7 +15258,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="4:8">
+    <row r="148" spans="4:8" ht="18">
       <c r="D148" s="12">
         <v>147</v>
       </c>
@@ -15264,7 +15275,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="149" spans="4:8">
+    <row r="149" spans="4:8" ht="18">
       <c r="D149" s="12">
         <v>148</v>
       </c>
@@ -15281,7 +15292,7 @@
         <v>1900021</v>
       </c>
     </row>
-    <row r="150" spans="4:8">
+    <row r="150" spans="4:8" ht="18">
       <c r="D150" s="12">
         <v>149</v>
       </c>
@@ -15298,7 +15309,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="151" spans="4:8">
+    <row r="151" spans="4:8" ht="18">
       <c r="D151" s="12">
         <v>150</v>
       </c>
@@ -15315,7 +15326,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="152" spans="4:8">
+    <row r="152" spans="4:8" ht="18">
       <c r="D152" s="12">
         <v>151</v>
       </c>
@@ -15332,7 +15343,7 @@
         <v>1900041</v>
       </c>
     </row>
-    <row r="153" spans="4:8">
+    <row r="153" spans="4:8" ht="18">
       <c r="D153" s="12">
         <v>152</v>
       </c>
@@ -15349,7 +15360,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="154" spans="4:8">
+    <row r="154" spans="4:8" ht="18">
       <c r="D154" s="12">
         <v>153</v>
       </c>
@@ -15366,7 +15377,7 @@
         <v>9532</v>
       </c>
     </row>
-    <row r="155" spans="4:8">
+    <row r="155" spans="4:8" ht="18">
       <c r="D155" s="12">
         <v>154</v>
       </c>
@@ -15383,7 +15394,7 @@
         <v>1900064</v>
       </c>
     </row>
-    <row r="156" spans="4:8">
+    <row r="156" spans="4:8" ht="18">
       <c r="D156" s="12">
         <v>155</v>
       </c>
@@ -15400,7 +15411,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="157" spans="4:8">
+    <row r="157" spans="4:8" ht="18">
       <c r="D157" s="12">
         <v>156</v>
       </c>
@@ -15417,7 +15428,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="158" spans="4:8">
+    <row r="158" spans="4:8" ht="18">
       <c r="D158" s="12">
         <v>157</v>
       </c>
@@ -15434,7 +15445,7 @@
         <v>1900062</v>
       </c>
     </row>
-    <row r="159" spans="4:8">
+    <row r="159" spans="4:8" ht="18">
       <c r="D159" s="12">
         <v>158</v>
       </c>
@@ -15451,7 +15462,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="160" spans="4:8">
+    <row r="160" spans="4:8" ht="18">
       <c r="D160" s="12">
         <v>159</v>
       </c>
@@ -15468,7 +15479,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="161" spans="4:8">
+    <row r="161" spans="4:8" ht="18">
       <c r="D161" s="12">
         <v>160</v>
       </c>
@@ -15485,7 +15496,7 @@
         <v>1900050</v>
       </c>
     </row>
-    <row r="162" spans="4:8">
+    <row r="162" spans="4:8" ht="18">
       <c r="D162" s="12">
         <v>161</v>
       </c>
@@ -15502,7 +15513,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="163" spans="4:8">
+    <row r="163" spans="4:8" ht="18">
       <c r="D163" s="12">
         <v>162</v>
       </c>
@@ -15519,7 +15530,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="164" spans="4:8">
+    <row r="164" spans="4:8" ht="18">
       <c r="D164" s="12">
         <v>163</v>
       </c>
@@ -15536,7 +15547,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="165" spans="4:8">
+    <row r="165" spans="4:8" ht="18">
       <c r="D165" s="12">
         <v>164</v>
       </c>
@@ -15553,7 +15564,7 @@
         <v>1900029</v>
       </c>
     </row>
-    <row r="166" spans="4:8">
+    <row r="166" spans="4:8" ht="18">
       <c r="D166" s="21">
         <v>165</v>
       </c>
@@ -15570,7 +15581,7 @@
         <v>1900028</v>
       </c>
     </row>
-    <row r="167" spans="4:8">
+    <row r="167" spans="4:8" ht="18">
       <c r="D167" s="12">
         <v>166</v>
       </c>
@@ -15587,7 +15598,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="168" spans="4:8">
+    <row r="168" spans="4:8" ht="18">
       <c r="D168" s="12">
         <v>167</v>
       </c>
@@ -15604,7 +15615,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="169" spans="4:8">
+    <row r="169" spans="4:8" ht="18">
       <c r="D169" s="12">
         <v>168</v>
       </c>
@@ -15621,7 +15632,7 @@
         <v>9462</v>
       </c>
     </row>
-    <row r="170" spans="4:8">
+    <row r="170" spans="4:8" ht="18">
       <c r="D170" s="12">
         <v>169</v>
       </c>
@@ -15638,7 +15649,7 @@
         <v>1900416</v>
       </c>
     </row>
-    <row r="171" spans="4:8">
+    <row r="171" spans="4:8" ht="18">
       <c r="D171" s="12">
         <v>170</v>
       </c>
@@ -15655,7 +15666,7 @@
         <v>4161</v>
       </c>
     </row>
-    <row r="172" spans="4:8">
+    <row r="172" spans="4:8" ht="18">
       <c r="D172" s="12">
         <v>171</v>
       </c>
@@ -15672,7 +15683,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="173" spans="4:8">
+    <row r="173" spans="4:8" ht="18">
       <c r="D173" s="12">
         <v>172</v>
       </c>
@@ -15689,7 +15700,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="174" spans="4:8">
+    <row r="174" spans="4:8" ht="18">
       <c r="D174" s="12">
         <v>173</v>
       </c>
@@ -15706,7 +15717,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="175" spans="4:8">
+    <row r="175" spans="4:8" ht="18">
       <c r="D175" s="12">
         <v>174</v>
       </c>
@@ -15723,7 +15734,7 @@
         <v>1900411</v>
       </c>
     </row>
-    <row r="176" spans="4:8">
+    <row r="176" spans="4:8" ht="18">
       <c r="D176" s="12">
         <v>175</v>
       </c>
@@ -15740,7 +15751,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="177" spans="4:8">
+    <row r="177" spans="4:8" ht="18">
       <c r="D177" s="12">
         <v>176</v>
       </c>
@@ -15757,7 +15768,7 @@
         <v>1900413</v>
       </c>
     </row>
-    <row r="178" spans="4:8">
+    <row r="178" spans="4:8" ht="18">
       <c r="D178" s="12">
         <v>177</v>
       </c>
@@ -15774,7 +15785,7 @@
         <v>1900415</v>
       </c>
     </row>
-    <row r="179" spans="4:8">
+    <row r="179" spans="4:8" ht="18">
       <c r="D179" s="12">
         <v>178</v>
       </c>
@@ -15791,7 +15802,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="180" spans="4:8">
+    <row r="180" spans="4:8" ht="18">
       <c r="D180" s="12">
         <v>179</v>
       </c>
@@ -15808,7 +15819,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="181" spans="4:8">
+    <row r="181" spans="4:8" ht="18">
       <c r="D181" s="12">
         <v>180</v>
       </c>
@@ -15825,7 +15836,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="182" spans="4:8">
+    <row r="182" spans="4:8" ht="18">
       <c r="D182" s="12">
         <v>181</v>
       </c>
@@ -15842,7 +15853,7 @@
         <v>4118</v>
       </c>
     </row>
-    <row r="183" spans="4:8">
+    <row r="183" spans="4:8" ht="18">
       <c r="D183" s="12">
         <v>182</v>
       </c>
@@ -15859,7 +15870,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="184" spans="4:8">
+    <row r="184" spans="4:8" ht="18">
       <c r="D184" s="12">
         <v>183</v>
       </c>
@@ -15876,7 +15887,7 @@
         <v>4165</v>
       </c>
     </row>
-    <row r="185" spans="4:8">
+    <row r="185" spans="4:8" ht="18">
       <c r="D185" s="21">
         <v>184</v>
       </c>
@@ -15893,7 +15904,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="186" spans="4:8">
+    <row r="186" spans="4:8" ht="18">
       <c r="D186" s="12">
         <v>185</v>
       </c>
@@ -15910,7 +15921,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="187" spans="4:8">
+    <row r="187" spans="4:8" ht="18">
       <c r="D187" s="12">
         <v>186</v>
       </c>
@@ -15927,7 +15938,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="188" spans="4:8">
+    <row r="188" spans="4:8" ht="18">
       <c r="D188" s="12">
         <v>187</v>
       </c>
@@ -15944,7 +15955,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="189" spans="4:8">
+    <row r="189" spans="4:8" ht="18">
       <c r="D189" s="12">
         <v>188</v>
       </c>
@@ -15961,7 +15972,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="190" spans="4:8">
+    <row r="190" spans="4:8" ht="18">
       <c r="D190" s="12">
         <v>189</v>
       </c>
@@ -15978,7 +15989,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="191" spans="4:8">
+    <row r="191" spans="4:8" ht="18">
       <c r="D191" s="12">
         <v>190</v>
       </c>
@@ -15995,7 +16006,7 @@
         <v>9547</v>
       </c>
     </row>
-    <row r="192" spans="4:8">
+    <row r="192" spans="4:8" ht="18">
       <c r="D192" s="12">
         <v>191</v>
       </c>
@@ -16012,7 +16023,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="193" spans="4:8">
+    <row r="193" spans="4:8" ht="18">
       <c r="D193" s="12">
         <v>192</v>
       </c>
@@ -16029,7 +16040,7 @@
         <v>4518</v>
       </c>
     </row>
-    <row r="194" spans="4:8">
+    <row r="194" spans="4:8" ht="18">
       <c r="D194" s="12">
         <v>193</v>
       </c>
@@ -16046,7 +16057,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="195" spans="4:8">
+    <row r="195" spans="4:8" ht="18">
       <c r="D195" s="12">
         <v>194</v>
       </c>
@@ -16063,7 +16074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="196" spans="4:8">
+    <row r="196" spans="4:8" ht="18">
       <c r="D196" s="12">
         <v>195</v>
       </c>
@@ -16080,7 +16091,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="197" spans="4:8">
+    <row r="197" spans="4:8" ht="18">
       <c r="D197" s="12">
         <v>196</v>
       </c>
@@ -16097,7 +16108,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="198" spans="4:8">
+    <row r="198" spans="4:8" ht="18">
       <c r="D198" s="12">
         <v>197</v>
       </c>
@@ -16114,7 +16125,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="199" spans="4:8">
+    <row r="199" spans="4:8" ht="18">
       <c r="D199" s="12">
         <v>198</v>
       </c>
@@ -16131,7 +16142,7 @@
         <v>1900194</v>
       </c>
     </row>
-    <row r="200" spans="4:8">
+    <row r="200" spans="4:8" ht="18">
       <c r="D200" s="12">
         <v>199</v>
       </c>
@@ -16148,7 +16159,7 @@
         <v>1900185</v>
       </c>
     </row>
-    <row r="201" spans="4:8">
+    <row r="201" spans="4:8" ht="18">
       <c r="D201" s="12">
         <v>200</v>
       </c>
@@ -16165,7 +16176,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="202" spans="4:8">
+    <row r="202" spans="4:8" ht="18">
       <c r="D202" s="12">
         <v>201</v>
       </c>
@@ -16182,7 +16193,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="203" spans="4:8">
+    <row r="203" spans="4:8" ht="18">
       <c r="D203" s="12">
         <v>202</v>
       </c>
@@ -16199,7 +16210,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="204" spans="4:8">
+    <row r="204" spans="4:8" ht="18">
       <c r="D204" s="12">
         <v>203</v>
       </c>
@@ -16216,7 +16227,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="205" spans="4:8">
+    <row r="205" spans="4:8" ht="18">
       <c r="D205" s="12">
         <v>204</v>
       </c>
@@ -16233,7 +16244,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="206" spans="4:8">
+    <row r="206" spans="4:8" ht="18">
       <c r="D206" s="12">
         <v>205</v>
       </c>
@@ -16250,7 +16261,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="207" spans="4:8">
+    <row r="207" spans="4:8" ht="18">
       <c r="D207" s="12">
         <v>206</v>
       </c>
@@ -16267,7 +16278,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="208" spans="4:8">
+    <row r="208" spans="4:8" ht="18">
       <c r="D208" s="12">
         <v>207</v>
       </c>
@@ -16284,7 +16295,7 @@
         <v>4532</v>
       </c>
     </row>
-    <row r="209" spans="4:8">
+    <row r="209" spans="4:8" ht="18">
       <c r="D209" s="12">
         <v>208</v>
       </c>
@@ -16301,7 +16312,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="210" spans="4:8">
+    <row r="210" spans="4:8" ht="18">
       <c r="D210" s="12">
         <v>209</v>
       </c>
@@ -16318,7 +16329,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="211" spans="4:8">
+    <row r="211" spans="4:8" ht="18">
       <c r="D211" s="12">
         <v>210</v>
       </c>
@@ -16335,7 +16346,7 @@
         <v>1900195</v>
       </c>
     </row>
-    <row r="212" spans="4:8">
+    <row r="212" spans="4:8" ht="18">
       <c r="D212" s="12">
         <v>211</v>
       </c>
@@ -16352,7 +16363,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="213" spans="4:8">
+    <row r="213" spans="4:8" ht="18">
       <c r="D213" s="12">
         <v>212</v>
       </c>
@@ -16369,7 +16380,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="214" spans="4:8">
+    <row r="214" spans="4:8" ht="18">
       <c r="D214" s="12">
         <v>213</v>
       </c>
@@ -16386,7 +16397,7 @@
         <v>1900196</v>
       </c>
     </row>
-    <row r="215" spans="4:8">
+    <row r="215" spans="4:8" ht="18">
       <c r="D215" s="12">
         <v>214</v>
       </c>
@@ -16403,7 +16414,7 @@
         <v>1900192</v>
       </c>
     </row>
-    <row r="216" spans="4:8">
+    <row r="216" spans="4:8" ht="18">
       <c r="D216" s="12">
         <v>215</v>
       </c>
@@ -16420,7 +16431,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="217" spans="4:8">
+    <row r="217" spans="4:8" ht="18">
       <c r="D217" s="12">
         <v>216</v>
       </c>
@@ -16437,7 +16448,7 @@
         <v>5241</v>
       </c>
     </row>
-    <row r="218" spans="4:8">
+    <row r="218" spans="4:8" ht="18">
       <c r="D218" s="12">
         <v>217</v>
       </c>
@@ -16454,7 +16465,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="219" spans="4:8">
+    <row r="219" spans="4:8" ht="18">
       <c r="D219" s="12">
         <v>218</v>
       </c>
@@ -16471,7 +16482,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="220" spans="4:8">
+    <row r="220" spans="4:8" ht="18">
       <c r="D220" s="12">
         <v>219</v>
       </c>
@@ -16488,7 +16499,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="221" spans="4:8">
+    <row r="221" spans="4:8" ht="18">
       <c r="D221" s="21">
         <v>220</v>
       </c>
@@ -16505,7 +16516,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="222" spans="4:8">
+    <row r="222" spans="4:8" ht="18">
       <c r="D222" s="12">
         <v>221</v>
       </c>
@@ -16522,7 +16533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="223" spans="4:8">
+    <row r="223" spans="4:8" ht="18">
       <c r="D223" s="12">
         <v>222</v>
       </c>
@@ -16539,7 +16550,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="224" spans="4:8">
+    <row r="224" spans="4:8" ht="18">
       <c r="D224" s="12">
         <v>223</v>
       </c>
@@ -16556,7 +16567,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="225" spans="4:8">
+    <row r="225" spans="4:8" ht="18">
       <c r="D225" s="12">
         <v>224</v>
       </c>
@@ -16573,7 +16584,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="226" spans="4:8">
+    <row r="226" spans="4:8" ht="18">
       <c r="D226" s="12">
         <v>225</v>
       </c>
@@ -16590,7 +16601,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="227" spans="4:8">
+    <row r="227" spans="4:8" ht="18">
       <c r="D227" s="12">
         <v>226</v>
       </c>
@@ -16607,7 +16618,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="228" spans="4:8">
+    <row r="228" spans="4:8" ht="18">
       <c r="D228" s="12">
         <v>227</v>
       </c>
@@ -16624,7 +16635,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="229" spans="4:8">
+    <row r="229" spans="4:8" ht="18">
       <c r="D229" s="12">
         <v>228</v>
       </c>
@@ -16641,7 +16652,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="230" spans="4:8">
+    <row r="230" spans="4:8" ht="18">
       <c r="D230" s="12">
         <v>229</v>
       </c>
@@ -16658,7 +16669,7 @@
         <v>5249</v>
       </c>
     </row>
-    <row r="231" spans="4:8">
+    <row r="231" spans="4:8" ht="18">
       <c r="D231" s="12">
         <v>230</v>
       </c>
@@ -16675,7 +16686,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="232" spans="4:8">
+    <row r="232" spans="4:8" ht="18">
       <c r="D232" s="12">
         <v>231</v>
       </c>
@@ -16692,7 +16703,7 @@
         <v>1900113</v>
       </c>
     </row>
-    <row r="233" spans="4:8">
+    <row r="233" spans="4:8" ht="18">
       <c r="D233" s="12">
         <v>232</v>
       </c>
@@ -16709,7 +16720,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="4:8">
+    <row r="234" spans="4:8" ht="18">
       <c r="D234" s="12">
         <v>233</v>
       </c>
@@ -16726,7 +16737,7 @@
         <v>1900112</v>
       </c>
     </row>
-    <row r="235" spans="4:8">
+    <row r="235" spans="4:8" ht="18">
       <c r="D235" s="12">
         <v>234</v>
       </c>
@@ -16743,7 +16754,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="236" spans="4:8">
+    <row r="236" spans="4:8" ht="18">
       <c r="D236" s="12">
         <v>235</v>
       </c>
@@ -16760,7 +16771,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="237" spans="4:8">
+    <row r="237" spans="4:8" ht="18">
       <c r="D237" s="12">
         <v>236</v>
       </c>
@@ -16777,7 +16788,7 @@
         <v>5001</v>
       </c>
     </row>
-    <row r="238" spans="4:8">
+    <row r="238" spans="4:8" ht="18">
       <c r="D238" s="21">
         <v>237</v>
       </c>
@@ -16794,7 +16805,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="239" spans="4:8">
+    <row r="239" spans="4:8" ht="18">
       <c r="D239" s="12">
         <v>238</v>
       </c>
@@ -16811,7 +16822,7 @@
         <v>4216</v>
       </c>
     </row>
-    <row r="240" spans="4:8">
+    <row r="240" spans="4:8" ht="18">
       <c r="D240" s="12">
         <v>239</v>
       </c>
@@ -16828,7 +16839,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="241" spans="4:8">
+    <row r="241" spans="4:8" ht="18">
       <c r="D241" s="12">
         <v>240</v>
       </c>
@@ -16845,7 +16856,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="242" spans="4:8">
+    <row r="242" spans="4:8" ht="18">
       <c r="D242" s="12">
         <v>241</v>
       </c>
@@ -16862,7 +16873,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="243" spans="4:8">
+    <row r="243" spans="4:8" ht="18">
       <c r="D243" s="12">
         <v>242</v>
       </c>
@@ -16879,7 +16890,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="244" spans="4:8">
+    <row r="244" spans="4:8" ht="18">
       <c r="D244" s="12">
         <v>243</v>
       </c>
@@ -16896,7 +16907,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="245" spans="4:8">
+    <row r="245" spans="4:8" ht="18">
       <c r="D245" s="12">
         <v>244</v>
       </c>
@@ -16913,7 +16924,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="246" spans="4:8">
+    <row r="246" spans="4:8" ht="18">
       <c r="D246" s="12">
         <v>245</v>
       </c>
@@ -16930,7 +16941,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="247" spans="4:8">
+    <row r="247" spans="4:8" ht="18">
       <c r="D247" s="12">
         <v>246</v>
       </c>
@@ -16947,7 +16958,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="248" spans="4:8">
+    <row r="248" spans="4:8" ht="18">
       <c r="D248" s="12">
         <v>247</v>
       </c>
@@ -16964,7 +16975,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="249" spans="4:8">
+    <row r="249" spans="4:8" ht="18">
       <c r="D249" s="12">
         <v>248</v>
       </c>
@@ -16981,7 +16992,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="250" spans="4:8">
+    <row r="250" spans="4:8" ht="18">
       <c r="D250" s="12">
         <v>249</v>
       </c>
@@ -16998,7 +17009,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="251" spans="4:8">
+    <row r="251" spans="4:8" ht="18">
       <c r="D251" s="12">
         <v>250</v>
       </c>
@@ -17015,7 +17026,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="252" spans="4:8">
+    <row r="252" spans="4:8" ht="18">
       <c r="D252" s="12">
         <v>251</v>
       </c>
@@ -17032,7 +17043,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="253" spans="4:8">
+    <row r="253" spans="4:8" ht="18">
       <c r="D253" s="12">
         <v>252</v>
       </c>
@@ -17049,7 +17060,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="254" spans="4:8">
+    <row r="254" spans="4:8" ht="18">
       <c r="D254" s="12">
         <v>253</v>
       </c>
@@ -17066,7 +17077,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="255" spans="4:8">
+    <row r="255" spans="4:8" ht="18">
       <c r="D255" s="12">
         <v>254</v>
       </c>
@@ -17083,7 +17094,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="256" spans="4:8">
+    <row r="256" spans="4:8" ht="18">
       <c r="D256" s="12">
         <v>255</v>
       </c>
@@ -17100,7 +17111,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="257" spans="4:8">
+    <row r="257" spans="4:8" ht="18">
       <c r="D257" s="12">
         <v>256</v>
       </c>
@@ -17117,7 +17128,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="258" spans="4:8">
+    <row r="258" spans="4:8" ht="18">
       <c r="D258" s="12">
         <v>257</v>
       </c>
@@ -17134,7 +17145,7 @@
         <v>6137</v>
       </c>
     </row>
-    <row r="259" spans="4:8">
+    <row r="259" spans="4:8" ht="18">
       <c r="D259" s="12">
         <v>258</v>
       </c>
@@ -17151,7 +17162,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="260" spans="4:8">
+    <row r="260" spans="4:8" ht="18">
       <c r="D260" s="12">
         <v>259</v>
       </c>
@@ -17168,7 +17179,7 @@
         <v>3619</v>
       </c>
     </row>
-    <row r="261" spans="4:8">
+    <row r="261" spans="4:8" ht="18">
       <c r="D261" s="12">
         <v>260</v>
       </c>
@@ -17185,7 +17196,7 @@
         <v>6128</v>
       </c>
     </row>
-    <row r="262" spans="4:8">
+    <row r="262" spans="4:8" ht="18">
       <c r="D262" s="12">
         <v>261</v>
       </c>
@@ -17202,7 +17213,7 @@
         <v>1900291</v>
       </c>
     </row>
-    <row r="263" spans="4:8">
+    <row r="263" spans="4:8" ht="18">
       <c r="D263" s="12">
         <v>262</v>
       </c>
@@ -17219,7 +17230,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="264" spans="4:8">
+    <row r="264" spans="4:8" ht="18">
       <c r="D264" s="12">
         <v>263</v>
       </c>
@@ -17236,7 +17247,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="265" spans="4:8">
+    <row r="265" spans="4:8" ht="18">
       <c r="D265" s="12">
         <v>264</v>
       </c>
@@ -17253,7 +17264,7 @@
         <v>3845</v>
       </c>
     </row>
-    <row r="266" spans="4:8">
+    <row r="266" spans="4:8" ht="18">
       <c r="D266" s="12">
         <v>265</v>
       </c>
@@ -17270,7 +17281,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="267" spans="4:8">
+    <row r="267" spans="4:8" ht="18">
       <c r="D267" s="12">
         <v>266</v>
       </c>
@@ -17287,7 +17298,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="268" spans="4:8">
+    <row r="268" spans="4:8" ht="18">
       <c r="D268" s="12">
         <v>267</v>
       </c>
@@ -17304,7 +17315,7 @@
         <v>1900290</v>
       </c>
     </row>
-    <row r="269" spans="4:8">
+    <row r="269" spans="4:8" ht="18">
       <c r="D269" s="12">
         <v>268</v>
       </c>
@@ -17321,7 +17332,7 @@
         <v>6238</v>
       </c>
     </row>
-    <row r="270" spans="4:8">
+    <row r="270" spans="4:8" ht="18">
       <c r="D270" s="12">
         <v>269</v>
       </c>
@@ -17338,7 +17349,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="271" spans="4:8">
+    <row r="271" spans="4:8" ht="18">
       <c r="D271" s="12">
         <v>270</v>
       </c>
@@ -17355,7 +17366,7 @@
         <v>6123</v>
       </c>
     </row>
-    <row r="272" spans="4:8">
+    <row r="272" spans="4:8" ht="18">
       <c r="D272" s="12">
         <v>271</v>
       </c>
@@ -17372,7 +17383,7 @@
         <v>1900289</v>
       </c>
     </row>
-    <row r="273" spans="4:8">
+    <row r="273" spans="4:8" ht="18">
       <c r="D273" s="12">
         <v>272</v>
       </c>
@@ -17389,7 +17400,7 @@
         <v>1900288</v>
       </c>
     </row>
-    <row r="274" spans="4:8">
+    <row r="274" spans="4:8" ht="18">
       <c r="D274" s="12">
         <v>273</v>
       </c>
@@ -17406,7 +17417,7 @@
         <v>5429</v>
       </c>
     </row>
-    <row r="275" spans="4:8">
+    <row r="275" spans="4:8" ht="18">
       <c r="D275" s="12">
         <v>274</v>
       </c>
@@ -17423,7 +17434,7 @@
         <v>1496</v>
       </c>
     </row>
-    <row r="276" spans="4:8">
+    <row r="276" spans="4:8" ht="18">
       <c r="D276" s="12">
         <v>275</v>
       </c>
@@ -17440,7 +17451,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="277" spans="4:8">
+    <row r="277" spans="4:8" ht="18">
       <c r="D277" s="12">
         <v>276</v>
       </c>
@@ -17457,7 +17468,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="278" spans="4:8">
+    <row r="278" spans="4:8" ht="18">
       <c r="D278" s="12">
         <v>277</v>
       </c>
@@ -17474,7 +17485,7 @@
         <v>3910</v>
       </c>
     </row>
-    <row r="279" spans="4:8">
+    <row r="279" spans="4:8" ht="18">
       <c r="D279" s="12">
         <v>278</v>
       </c>
@@ -17491,7 +17502,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="280" spans="4:8">
+    <row r="280" spans="4:8" ht="18">
       <c r="D280" s="12">
         <v>279</v>
       </c>
@@ -17508,7 +17519,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="281" spans="4:8">
+    <row r="281" spans="4:8" ht="18">
       <c r="D281" s="12">
         <v>280</v>
       </c>
@@ -17525,7 +17536,7 @@
         <v>8498</v>
       </c>
     </row>
-    <row r="282" spans="4:8">
+    <row r="282" spans="4:8" ht="18">
       <c r="D282" s="12">
         <v>281</v>
       </c>
@@ -17542,7 +17553,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="283" spans="4:8">
+    <row r="283" spans="4:8" ht="18">
       <c r="D283" s="12">
         <v>282</v>
       </c>
@@ -17559,7 +17570,7 @@
         <v>5466</v>
       </c>
     </row>
-    <row r="284" spans="4:8">
+    <row r="284" spans="4:8" ht="18">
       <c r="D284" s="12">
         <v>283</v>
       </c>
@@ -17576,7 +17587,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="285" spans="4:8">
+    <row r="285" spans="4:8" ht="18">
       <c r="D285" s="12">
         <v>284</v>
       </c>
@@ -17593,7 +17604,7 @@
         <v>5483</v>
       </c>
     </row>
-    <row r="286" spans="4:8">
+    <row r="286" spans="4:8" ht="18">
       <c r="D286" s="12">
         <v>285</v>
       </c>
@@ -17610,7 +17621,7 @@
         <v>5919</v>
       </c>
     </row>
-    <row r="287" spans="4:8">
+    <row r="287" spans="4:8" ht="18">
       <c r="D287" s="12">
         <v>286</v>
       </c>
@@ -17627,7 +17638,7 @@
         <v>3649</v>
       </c>
     </row>
-    <row r="288" spans="4:8">
+    <row r="288" spans="4:8" ht="18">
       <c r="D288" s="12">
         <v>287</v>
       </c>
@@ -17644,7 +17655,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="289" spans="4:8">
+    <row r="289" spans="4:8" ht="18">
       <c r="D289" s="12">
         <v>288</v>
       </c>
@@ -17661,7 +17672,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="290" spans="4:8">
+    <row r="290" spans="4:8" ht="18">
       <c r="D290" s="12">
         <v>289</v>
       </c>
@@ -17678,7 +17689,7 @@
         <v>6121</v>
       </c>
     </row>
-    <row r="291" spans="4:8">
+    <row r="291" spans="4:8" ht="18">
       <c r="D291" s="12">
         <v>290</v>
       </c>
@@ -17695,7 +17706,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="292" spans="4:8">
+    <row r="292" spans="4:8" ht="18">
       <c r="D292" s="12">
         <v>291</v>
       </c>
@@ -17712,7 +17723,7 @@
         <v>5968</v>
       </c>
     </row>
-    <row r="293" spans="4:8">
+    <row r="293" spans="4:8" ht="18">
       <c r="D293" s="12">
         <v>292</v>
       </c>
@@ -17729,7 +17740,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="294" spans="4:8">
+    <row r="294" spans="4:8" ht="18">
       <c r="D294" s="12">
         <v>293</v>
       </c>
@@ -17746,7 +17757,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="295" spans="4:8">
+    <row r="295" spans="4:8" ht="18">
       <c r="D295" s="12">
         <v>294</v>
       </c>
@@ -17763,7 +17774,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="296" spans="4:8">
+    <row r="296" spans="4:8" ht="18">
       <c r="D296" s="12">
         <v>295</v>
       </c>
@@ -17780,7 +17791,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="297" spans="4:8">
+    <row r="297" spans="4:8" ht="18">
       <c r="D297" s="12">
         <v>296</v>
       </c>
@@ -17797,7 +17808,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="298" spans="4:8">
+    <row r="298" spans="4:8" ht="18">
       <c r="D298" s="12">
         <v>297</v>
       </c>
@@ -17814,7 +17825,7 @@
         <v>5961</v>
       </c>
     </row>
-    <row r="299" spans="4:8">
+    <row r="299" spans="4:8" ht="18">
       <c r="D299" s="12">
         <v>298</v>
       </c>
@@ -17831,7 +17842,7 @@
         <v>1900292</v>
       </c>
     </row>
-    <row r="300" spans="4:8">
+    <row r="300" spans="4:8" ht="18">
       <c r="D300" s="12">
         <v>299</v>
       </c>
@@ -17848,7 +17859,7 @@
         <v>3626</v>
       </c>
     </row>
-    <row r="301" spans="4:8">
+    <row r="301" spans="4:8" ht="18">
       <c r="D301" s="12">
         <v>300</v>
       </c>
@@ -17865,7 +17876,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="302" spans="4:8">
+    <row r="302" spans="4:8" ht="18">
       <c r="D302" s="12">
         <v>301</v>
       </c>
@@ -17882,7 +17893,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="303" spans="4:8">
+    <row r="303" spans="4:8" ht="18">
       <c r="D303" s="12">
         <v>302</v>
       </c>
@@ -17899,7 +17910,7 @@
         <v>8494</v>
       </c>
     </row>
-    <row r="304" spans="4:8">
+    <row r="304" spans="4:8" ht="18">
       <c r="D304" s="12">
         <v>303</v>
       </c>
@@ -17916,7 +17927,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="305" spans="4:8">
+    <row r="305" spans="4:8" ht="18">
       <c r="D305" s="21">
         <v>304</v>
       </c>
@@ -17933,7 +17944,7 @@
         <v>3843</v>
       </c>
     </row>
-    <row r="306" spans="4:8">
+    <row r="306" spans="4:8" ht="18">
       <c r="D306" s="12">
         <v>305</v>
       </c>
@@ -17950,7 +17961,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="307" spans="4:8">
+    <row r="307" spans="4:8" ht="18">
       <c r="D307" s="12">
         <v>306</v>
       </c>
@@ -17967,7 +17978,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="308" spans="4:8">
+    <row r="308" spans="4:8" ht="18">
       <c r="D308" s="12">
         <v>307</v>
       </c>
@@ -17984,7 +17995,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="309" spans="4:8">
+    <row r="309" spans="4:8" ht="18">
       <c r="D309" s="12">
         <v>308</v>
       </c>
@@ -18001,7 +18012,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="310" spans="4:8">
+    <row r="310" spans="4:8" ht="18">
       <c r="D310" s="12">
         <v>309</v>
       </c>
@@ -18018,7 +18029,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="311" spans="4:8">
+    <row r="311" spans="4:8" ht="18">
       <c r="D311" s="12">
         <v>310</v>
       </c>
@@ -18035,7 +18046,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="312" spans="4:8">
+    <row r="312" spans="4:8" ht="18">
       <c r="D312" s="21">
         <v>311</v>
       </c>
@@ -18052,7 +18063,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="313" spans="4:8">
+    <row r="313" spans="4:8" ht="18">
       <c r="D313" s="12">
         <v>312</v>
       </c>
@@ -18069,7 +18080,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="314" spans="4:8">
+    <row r="314" spans="4:8" ht="18">
       <c r="D314" s="12">
         <v>313</v>
       </c>
@@ -18086,7 +18097,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="315" spans="4:8">
+    <row r="315" spans="4:8" ht="18">
       <c r="D315" s="12">
         <v>314</v>
       </c>
@@ -18103,7 +18114,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="316" spans="4:8">
+    <row r="316" spans="4:8" ht="18">
       <c r="D316" s="12">
         <v>315</v>
       </c>
@@ -18120,7 +18131,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="317" spans="4:8">
+    <row r="317" spans="4:8" ht="18">
       <c r="D317" s="12">
         <v>316</v>
       </c>
@@ -18137,7 +18148,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="318" spans="4:8">
+    <row r="318" spans="4:8" ht="18">
       <c r="D318" s="12">
         <v>317</v>
       </c>
@@ -18154,7 +18165,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="319" spans="4:8">
+    <row r="319" spans="4:8" ht="18">
       <c r="D319" s="12">
         <v>318</v>
       </c>
@@ -18171,7 +18182,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="320" spans="4:8">
+    <row r="320" spans="4:8" ht="18">
       <c r="D320" s="12">
         <v>319</v>
       </c>
@@ -18188,7 +18199,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="321" spans="4:8">
+    <row r="321" spans="4:8" ht="18">
       <c r="D321" s="12">
         <v>320</v>
       </c>
@@ -18205,7 +18216,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="322" spans="4:8">
+    <row r="322" spans="4:8" ht="18">
       <c r="D322" s="12">
         <v>321</v>
       </c>
@@ -18222,7 +18233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="323" spans="4:8">
+    <row r="323" spans="4:8" ht="18">
       <c r="D323" s="12">
         <v>322</v>
       </c>
@@ -18239,7 +18250,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="324" spans="4:8">
+    <row r="324" spans="4:8" ht="18">
       <c r="D324" s="12">
         <v>323</v>
       </c>
@@ -18256,7 +18267,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="325" spans="4:8">
+    <row r="325" spans="4:8" ht="18">
       <c r="D325" s="12">
         <v>324</v>
       </c>
@@ -18273,7 +18284,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="326" spans="4:8">
+    <row r="326" spans="4:8" ht="18">
       <c r="D326" s="12">
         <v>325</v>
       </c>
@@ -18290,7 +18301,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="327" spans="4:8">
+    <row r="327" spans="4:8" ht="18">
       <c r="D327" s="12">
         <v>326</v>
       </c>
@@ -18307,7 +18318,7 @@
         <v>9541</v>
       </c>
     </row>
-    <row r="328" spans="4:8">
+    <row r="328" spans="4:8" ht="18">
       <c r="D328" s="12">
         <v>327</v>
       </c>
@@ -18324,7 +18335,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="329" spans="4:8">
+    <row r="329" spans="4:8" ht="18">
       <c r="D329" s="21">
         <v>328</v>
       </c>
@@ -18341,7 +18352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="330" spans="4:8">
+    <row r="330" spans="4:8" ht="18">
       <c r="D330" s="12">
         <v>329</v>
       </c>
@@ -18358,7 +18369,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="331" spans="4:8">
+    <row r="331" spans="4:8" ht="18">
       <c r="D331" s="12">
         <v>330</v>
       </c>
@@ -18375,7 +18386,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="332" spans="4:8">
+    <row r="332" spans="4:8" ht="18">
       <c r="D332" s="12">
         <v>331</v>
       </c>
@@ -18392,7 +18403,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="333" spans="4:8">
+    <row r="333" spans="4:8" ht="18">
       <c r="D333" s="12">
         <v>332</v>
       </c>
@@ -18409,7 +18420,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="334" spans="4:8">
+    <row r="334" spans="4:8" ht="18">
       <c r="D334" s="12">
         <v>333</v>
       </c>
@@ -18426,7 +18437,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="335" spans="4:8">
+    <row r="335" spans="4:8" ht="18">
       <c r="D335" s="12">
         <v>334</v>
       </c>
@@ -18443,7 +18454,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="336" spans="4:8">
+    <row r="336" spans="4:8" ht="18">
       <c r="D336" s="12">
         <v>335</v>
       </c>
@@ -18460,7 +18471,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="337" spans="4:8">
+    <row r="337" spans="4:8" ht="18">
       <c r="D337" s="12">
         <v>336</v>
       </c>
@@ -18477,7 +18488,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="338" spans="4:8">
+    <row r="338" spans="4:8" ht="18">
       <c r="D338" s="12">
         <v>337</v>
       </c>
@@ -18494,7 +18505,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="339" spans="4:8">
+    <row r="339" spans="4:8" ht="18">
       <c r="D339" s="12">
         <v>338</v>
       </c>
@@ -18511,7 +18522,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="340" spans="4:8">
+    <row r="340" spans="4:8" ht="18">
       <c r="D340" s="12">
         <v>339</v>
       </c>
@@ -18528,7 +18539,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="341" spans="4:8">
+    <row r="341" spans="4:8" ht="18">
       <c r="D341" s="12">
         <v>340</v>
       </c>
@@ -18545,7 +18556,7 @@
         <v>5787</v>
       </c>
     </row>
-    <row r="342" spans="4:8">
+    <row r="342" spans="4:8" ht="18">
       <c r="D342" s="12">
         <v>341</v>
       </c>
@@ -18562,7 +18573,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="343" spans="4:8">
+    <row r="343" spans="4:8" ht="18">
       <c r="D343" s="12">
         <v>342</v>
       </c>
@@ -18579,7 +18590,7 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="344" spans="4:8">
+    <row r="344" spans="4:8" ht="18">
       <c r="D344" s="12">
         <v>343</v>
       </c>
@@ -18596,7 +18607,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="345" spans="4:8">
+    <row r="345" spans="4:8" ht="18">
       <c r="D345" s="12">
         <v>344</v>
       </c>
@@ -18613,7 +18624,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="346" spans="4:8">
+    <row r="346" spans="4:8" ht="18">
       <c r="D346" s="12">
         <v>345</v>
       </c>
@@ -18630,7 +18641,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="347" spans="4:8">
+    <row r="347" spans="4:8" ht="18">
       <c r="D347" s="12">
         <v>346</v>
       </c>
@@ -18647,7 +18658,7 @@
         <v>4247</v>
       </c>
     </row>
-    <row r="348" spans="4:8">
+    <row r="348" spans="4:8" ht="18">
       <c r="D348" s="12">
         <v>347</v>
       </c>
@@ -18664,7 +18675,7 @@
         <v>2855</v>
       </c>
     </row>
-    <row r="349" spans="4:8">
+    <row r="349" spans="4:8" ht="18">
       <c r="D349" s="12">
         <v>348</v>
       </c>
@@ -18681,7 +18692,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="350" spans="4:8">
+    <row r="350" spans="4:8" ht="18">
       <c r="D350" s="21">
         <v>349</v>
       </c>
@@ -18698,7 +18709,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="351" spans="4:8">
+    <row r="351" spans="4:8" ht="18">
       <c r="D351" s="12">
         <v>350</v>
       </c>
@@ -18715,7 +18726,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="352" spans="4:8">
+    <row r="352" spans="4:8" ht="18">
       <c r="D352" s="12">
         <v>351</v>
       </c>
@@ -18732,7 +18743,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="353" spans="4:8">
+    <row r="353" spans="4:8" ht="18">
       <c r="D353" s="12">
         <v>352</v>
       </c>
@@ -18749,7 +18760,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="354" spans="4:8">
+    <row r="354" spans="4:8" ht="18">
       <c r="D354" s="12">
         <v>353</v>
       </c>
@@ -18766,7 +18777,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="355" spans="4:8">
+    <row r="355" spans="4:8" ht="18">
       <c r="D355" s="12">
         <v>354</v>
       </c>
@@ -18783,7 +18794,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="356" spans="4:8">
+    <row r="356" spans="4:8" ht="18">
       <c r="D356" s="12">
         <v>355</v>
       </c>
@@ -18800,7 +18811,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="357" spans="4:8">
+    <row r="357" spans="4:8" ht="18">
       <c r="D357" s="12">
         <v>356</v>
       </c>
@@ -18817,7 +18828,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="358" spans="4:8">
+    <row r="358" spans="4:8" ht="18">
       <c r="D358" s="12">
         <v>357</v>
       </c>
@@ -18834,7 +18845,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="359" spans="4:8">
+    <row r="359" spans="4:8" ht="18">
       <c r="D359" s="12">
         <v>358</v>
       </c>
@@ -18851,7 +18862,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="360" spans="4:8">
+    <row r="360" spans="4:8" ht="18">
       <c r="D360" s="12">
         <v>359</v>
       </c>
@@ -18868,7 +18879,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="361" spans="4:8">
+    <row r="361" spans="4:8" ht="18">
       <c r="D361" s="12">
         <v>360</v>
       </c>
@@ -18885,7 +18896,7 @@
         <v>1900393</v>
       </c>
     </row>
-    <row r="362" spans="4:8">
+    <row r="362" spans="4:8" ht="18">
       <c r="D362" s="21">
         <v>361</v>
       </c>
@@ -18902,7 +18913,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="363" spans="4:8">
+    <row r="363" spans="4:8" ht="18">
       <c r="D363" s="12">
         <v>362</v>
       </c>
@@ -18919,7 +18930,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="364" spans="4:8">
+    <row r="364" spans="4:8" ht="18">
       <c r="D364" s="12">
         <v>363</v>
       </c>
@@ -18936,7 +18947,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="365" spans="4:8">
+    <row r="365" spans="4:8" ht="18">
       <c r="D365" s="12">
         <v>364</v>
       </c>
@@ -18953,7 +18964,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="366" spans="4:8">
+    <row r="366" spans="4:8" ht="18">
       <c r="D366" s="12">
         <v>365</v>
       </c>
@@ -18970,7 +18981,7 @@
         <v>3656</v>
       </c>
     </row>
-    <row r="367" spans="4:8">
+    <row r="367" spans="4:8" ht="18">
       <c r="D367" s="12">
         <v>366</v>
       </c>
@@ -18987,7 +18998,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="368" spans="4:8">
+    <row r="368" spans="4:8" ht="18">
       <c r="D368" s="12">
         <v>367</v>
       </c>
@@ -19004,7 +19015,7 @@
         <v>1900342</v>
       </c>
     </row>
-    <row r="369" spans="4:8">
+    <row r="369" spans="4:8" ht="18">
       <c r="D369" s="12">
         <v>368</v>
       </c>
@@ -19021,7 +19032,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="370" spans="4:8">
+    <row r="370" spans="4:8" ht="18">
       <c r="D370" s="12">
         <v>369</v>
       </c>
@@ -19038,7 +19049,7 @@
         <v>3695</v>
       </c>
     </row>
-    <row r="371" spans="4:8">
+    <row r="371" spans="4:8" ht="18">
       <c r="D371" s="12">
         <v>370</v>
       </c>
@@ -19055,7 +19066,7 @@
         <v>5872</v>
       </c>
     </row>
-    <row r="372" spans="4:8">
+    <row r="372" spans="4:8" ht="18">
       <c r="D372" s="12">
         <v>371</v>
       </c>
@@ -19072,7 +19083,7 @@
         <v>1341</v>
       </c>
     </row>
-    <row r="373" spans="4:8">
+    <row r="373" spans="4:8" ht="18">
       <c r="D373" s="12">
         <v>372</v>
       </c>
@@ -19089,7 +19100,7 @@
         <v>1900333</v>
       </c>
     </row>
-    <row r="374" spans="4:8">
+    <row r="374" spans="4:8" ht="18">
       <c r="D374" s="12">
         <v>373</v>
       </c>
@@ -19106,7 +19117,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="375" spans="4:8">
+    <row r="375" spans="4:8" ht="18">
       <c r="D375" s="12">
         <v>374</v>
       </c>
@@ -19123,7 +19134,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="376" spans="4:8">
+    <row r="376" spans="4:8" ht="18">
       <c r="D376" s="12">
         <v>375</v>
       </c>
@@ -19140,7 +19151,7 @@
         <v>1900337</v>
       </c>
     </row>
-    <row r="377" spans="4:8">
+    <row r="377" spans="4:8" ht="18">
       <c r="D377" s="12">
         <v>376</v>
       </c>
@@ -19157,7 +19168,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="378" spans="4:8">
+    <row r="378" spans="4:8" ht="18">
       <c r="D378" s="12">
         <v>377</v>
       </c>
@@ -19174,7 +19185,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="379" spans="4:8">
+    <row r="379" spans="4:8" ht="18">
       <c r="D379" s="12">
         <v>378</v>
       </c>
@@ -19191,7 +19202,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="380" spans="4:8">
+    <row r="380" spans="4:8" ht="18">
       <c r="D380" s="12">
         <v>379</v>
       </c>
@@ -19208,7 +19219,7 @@
         <v>5192</v>
       </c>
     </row>
-    <row r="381" spans="4:8">
+    <row r="381" spans="4:8" ht="18">
       <c r="D381" s="12">
         <v>380</v>
       </c>
@@ -19225,7 +19236,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="382" spans="4:8">
+    <row r="382" spans="4:8" ht="18">
       <c r="D382" s="21">
         <v>381</v>
       </c>
@@ -19242,7 +19253,7 @@
         <v>3618</v>
       </c>
     </row>
-    <row r="383" spans="4:8">
+    <row r="383" spans="4:8" ht="18">
       <c r="D383" s="12">
         <v>382</v>
       </c>
@@ -19259,7 +19270,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="384" spans="4:8">
+    <row r="384" spans="4:8" ht="18">
       <c r="D384" s="12">
         <v>383</v>
       </c>
@@ -19276,7 +19287,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="385" spans="4:8">
+    <row r="385" spans="4:8" ht="18">
       <c r="D385" s="12">
         <v>384</v>
       </c>
@@ -19293,7 +19304,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="386" spans="4:8">
+    <row r="386" spans="4:8" ht="18">
       <c r="D386" s="12">
         <v>385</v>
       </c>
@@ -19310,7 +19321,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="387" spans="4:8">
+    <row r="387" spans="4:8" ht="18">
       <c r="D387" s="21">
         <v>386</v>
       </c>
@@ -19327,7 +19338,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="388" spans="4:8">
+    <row r="388" spans="4:8" ht="18">
       <c r="D388" s="12">
         <v>387</v>
       </c>
@@ -19344,7 +19355,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="389" spans="4:8">
+    <row r="389" spans="4:8" ht="18">
       <c r="D389" s="12">
         <v>388</v>
       </c>
@@ -19361,7 +19372,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="390" spans="4:8">
+    <row r="390" spans="4:8" ht="18">
       <c r="D390" s="12">
         <v>389</v>
       </c>
@@ -19378,7 +19389,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="391" spans="4:8">
+    <row r="391" spans="4:8" ht="18">
       <c r="D391" s="12">
         <v>390</v>
       </c>
@@ -19395,7 +19406,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="392" spans="4:8">
+    <row r="392" spans="4:8" ht="18">
       <c r="D392" s="12">
         <v>391</v>
       </c>
@@ -19412,7 +19423,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="393" spans="4:8">
+    <row r="393" spans="4:8" ht="18">
       <c r="D393" s="12">
         <v>392</v>
       </c>
@@ -19429,7 +19440,7 @@
         <v>1667</v>
       </c>
     </row>
-    <row r="394" spans="4:8">
+    <row r="394" spans="4:8" ht="18">
       <c r="D394" s="12">
         <v>393</v>
       </c>
@@ -19446,7 +19457,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="395" spans="4:8">
+    <row r="395" spans="4:8" ht="18">
       <c r="D395" s="12">
         <v>394</v>
       </c>
@@ -19463,7 +19474,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="396" spans="4:8">
+    <row r="396" spans="4:8" ht="18">
       <c r="D396" s="12">
         <v>395</v>
       </c>
@@ -19480,7 +19491,7 @@
         <v>4504</v>
       </c>
     </row>
-    <row r="397" spans="4:8">
+    <row r="397" spans="4:8" ht="18">
       <c r="D397" s="12">
         <v>396</v>
       </c>
@@ -19497,7 +19508,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="398" spans="4:8">
+    <row r="398" spans="4:8" ht="18">
       <c r="D398" s="12">
         <v>397</v>
       </c>
@@ -19514,7 +19525,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="399" spans="4:8">
+    <row r="399" spans="4:8" ht="18">
       <c r="D399" s="12">
         <v>398</v>
       </c>
@@ -19531,7 +19542,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="400" spans="4:8">
+    <row r="400" spans="4:8" ht="18">
       <c r="D400" s="12">
         <v>399</v>
       </c>
@@ -19548,7 +19559,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="401" spans="4:8">
+    <row r="401" spans="4:8" ht="18">
       <c r="D401" s="12">
         <v>400</v>
       </c>
@@ -19565,7 +19576,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="402" spans="4:8">
+    <row r="402" spans="4:8" ht="18">
       <c r="D402" s="12">
         <v>401</v>
       </c>
@@ -19582,7 +19593,7 @@
         <v>4331</v>
       </c>
     </row>
-    <row r="403" spans="4:8">
+    <row r="403" spans="4:8" ht="18">
       <c r="D403" s="12">
         <v>402</v>
       </c>
@@ -19599,7 +19610,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="404" spans="4:8">
+    <row r="404" spans="4:8" ht="18">
       <c r="D404" s="12">
         <v>403</v>
       </c>
@@ -19616,7 +19627,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="405" spans="4:8">
+    <row r="405" spans="4:8" ht="18">
       <c r="D405" s="12">
         <v>404</v>
       </c>
@@ -19633,7 +19644,7 @@
         <v>1900308</v>
       </c>
     </row>
-    <row r="406" spans="4:8">
+    <row r="406" spans="4:8" ht="18">
       <c r="D406" s="12">
         <v>405</v>
       </c>
@@ -19650,7 +19661,7 @@
         <v>4480</v>
       </c>
     </row>
-    <row r="407" spans="4:8">
+    <row r="407" spans="4:8" ht="18">
       <c r="D407" s="12">
         <v>406</v>
       </c>
@@ -19667,7 +19678,7 @@
         <v>4441</v>
       </c>
     </row>
-    <row r="408" spans="4:8">
+    <row r="408" spans="4:8" ht="18">
       <c r="D408" s="12">
         <v>407</v>
       </c>
@@ -19684,7 +19695,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="409" spans="4:8">
+    <row r="409" spans="4:8" ht="18">
       <c r="D409" s="12">
         <v>408</v>
       </c>
@@ -19701,7 +19712,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="410" spans="4:8">
+    <row r="410" spans="4:8" ht="18">
       <c r="D410" s="21">
         <v>409</v>
       </c>
@@ -19718,7 +19729,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="411" spans="4:8">
+    <row r="411" spans="4:8" ht="18">
       <c r="D411" s="12">
         <v>410</v>
       </c>
@@ -19735,7 +19746,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="412" spans="4:8">
+    <row r="412" spans="4:8" ht="18">
       <c r="D412" s="12">
         <v>411</v>
       </c>
@@ -19752,7 +19763,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="413" spans="4:8">
+    <row r="413" spans="4:8" ht="18">
       <c r="D413" s="12">
         <v>412</v>
       </c>
@@ -19769,7 +19780,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="414" spans="4:8">
+    <row r="414" spans="4:8" ht="18">
       <c r="D414" s="12">
         <v>413</v>
       </c>
@@ -19786,7 +19797,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="415" spans="4:8">
+    <row r="415" spans="4:8" ht="18">
       <c r="D415" s="12">
         <v>414</v>
       </c>
@@ -19803,7 +19814,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="416" spans="4:8">
+    <row r="416" spans="4:8" ht="18">
       <c r="D416" s="12">
         <v>415</v>
       </c>
@@ -19820,7 +19831,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="417" spans="4:8">
+    <row r="417" spans="4:8" ht="18">
       <c r="D417" s="12">
         <v>416</v>
       </c>
@@ -19837,7 +19848,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="418" spans="4:8">
+    <row r="418" spans="4:8" ht="18">
       <c r="D418" s="12">
         <v>417</v>
       </c>
@@ -19854,7 +19865,7 @@
         <v>5777</v>
       </c>
     </row>
-    <row r="419" spans="4:8">
+    <row r="419" spans="4:8" ht="18">
       <c r="D419" s="12">
         <v>418</v>
       </c>
@@ -19871,7 +19882,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="420" spans="4:8">
+    <row r="420" spans="4:8" ht="18">
       <c r="D420" s="12">
         <v>419</v>
       </c>
@@ -19888,7 +19899,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="421" spans="4:8" ht="17.25" thickBot="1">
+    <row r="421" spans="4:8" ht="19" thickBot="1">
       <c r="D421" s="15">
         <v>420</v>
       </c>
@@ -19915,21 +19926,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9D87A3-6C1F-4567-9B3F-F647653EDC46}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="11.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.75" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
     <col min="10" max="10" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -19967,11 +19978,11 @@
       <c r="K1" s="31" t="s">
         <v>545</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="35" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="54">
       <c r="A2" s="5">
         <v>1</v>
       </c>

</xml_diff>